<commit_message>
Test on new Azure AD app
</commit_message>
<xml_diff>
--- a/Configuration Specification.xlsx
+++ b/Configuration Specification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DavidBaker\source\repos\Dev\FC365_NPP_Dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DavidBaker\source\repos\Dev\FC365\FC365 NPP Dev-Test\npp-angular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B4877C-42C2-447C-AEEF-E1C4F79E7E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7500D6-A8BD-485B-A5F8-26F24C46FD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5235" yWindow="6975" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{28B7ACA7-9682-41CB-8AE6-FF1EA1DE0FC2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{28B7ACA7-9682-41CB-8AE6-FF1EA1DE0FC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Site" sheetId="3" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="220">
   <si>
     <t>Name</t>
   </si>
@@ -711,10 +711,34 @@
     <t>OpportunityGeography</t>
   </si>
   <si>
-    <t>https://janddconsulting.sharepoint.com/sites/FC365NPPDev</t>
-  </si>
-  <si>
     <t>GroupsToKeep</t>
+  </si>
+  <si>
+    <t>Master Power BI</t>
+  </si>
+  <si>
+    <t>GroupId</t>
+  </si>
+  <si>
+    <t>pageName</t>
+  </si>
+  <si>
+    <t>Master Power BI Components</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>ComponentType</t>
+  </si>
+  <si>
+    <t>ComponentOrder</t>
+  </si>
+  <si>
+    <t>ReportType</t>
+  </si>
+  <si>
+    <t>https://janddconsulting.sharepoint.com/sites/FC365NPPTest</t>
   </si>
 </sst>
 </file>
@@ -835,7 +859,33 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="7" tint="-0.24994659260841701"/>
@@ -843,16 +893,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
         </patternFill>
       </fill>
     </dxf>
@@ -926,32 +966,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -975,7 +989,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7ED3C973-7A1D-409F-8F7D-9D03D5B8CFC5}" name="tblLIstTemplates" displayName="tblLIstTemplates" ref="A1:A9" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7ED3C973-7A1D-409F-8F7D-9D03D5B8CFC5}" name="tblLIstTemplates" displayName="tblLIstTemplates" ref="A1:A9" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:A9" xr:uid="{7ED3C973-7A1D-409F-8F7D-9D03D5B8CFC5}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{B522FA47-3F00-4AE2-AD51-94952026AAAA}" name="List Templates"/>
@@ -985,7 +999,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{97D2B957-2728-4F3F-AF73-9CBED900FD28}" name="tblSiteColumns" displayName="tblSiteColumns" ref="C1:C14" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{97D2B957-2728-4F3F-AF73-9CBED900FD28}" name="tblSiteColumns" displayName="tblSiteColumns" ref="C1:C14" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="C1:C14" xr:uid="{97D2B957-2728-4F3F-AF73-9CBED900FD28}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{B9AF5774-4F7B-4EFB-A7A5-BC2D8EE820B1}" name="User Columns"/>
@@ -1325,8 +1339,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1340,13 +1354,16 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>210</v>
+      <c r="A2" s="11" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5F7F12CD-1AC2-46F5-A44E-0979F2898032}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3555,10 +3572,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B26AF0-04C3-407C-9D2A-5BC9525D0AFE}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3576,7 +3593,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>12</v>
@@ -3715,6 +3732,22 @@
         <v>153</v>
       </c>
       <c r="B18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3734,10 +3767,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4316C6F5-4268-4972-A50D-9F497A0970C5}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4516,34 +4549,142 @@
         <v>126</v>
       </c>
     </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>212</v>
+      </c>
+      <c r="B39" t="s">
+        <v>212</v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" t="s">
+        <v>124</v>
+      </c>
+      <c r="E39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>213</v>
+      </c>
+      <c r="B40" t="s">
+        <v>213</v>
+      </c>
+      <c r="C40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>215</v>
+      </c>
+      <c r="B41" t="s">
+        <v>215</v>
+      </c>
+      <c r="C41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" t="s">
+        <v>124</v>
+      </c>
+      <c r="E41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>216</v>
+      </c>
+      <c r="B42" t="s">
+        <v>216</v>
+      </c>
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" t="s">
+        <v>124</v>
+      </c>
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>217</v>
+      </c>
+      <c r="B43" t="s">
+        <v>217</v>
+      </c>
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" t="s">
+        <v>124</v>
+      </c>
+      <c r="E43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>218</v>
+      </c>
+      <c r="B44" t="s">
+        <v>218</v>
+      </c>
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" t="s">
+        <v>48</v>
+      </c>
+      <c r="J44" t="s">
+        <v>211</v>
+      </c>
+      <c r="K44" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>AND($C1="Yes/No",ISBLANK($F1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>AND($C1="Number",ISBLANK($G1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>AND(LEFT($C1,15)="User (Multiple)",ISBLANK($H1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>AND($C1="Choice",ISBLANK($I1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>AND(OR($C1="Lookup",$C1="LookupMulti"),ISBLANK($J1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>AND(OR($C1="Lookup",$C1="LookupMulti"),ISBLANK($K1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4576,10 +4717,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E230680E-7D77-4793-98FC-F33907744311}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4978,6 +5119,70 @@
       </c>
       <c r="B49" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>211</v>
+      </c>
+      <c r="B50" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>211</v>
+      </c>
+      <c r="B51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>211</v>
+      </c>
+      <c r="B52" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>211</v>
+      </c>
+      <c r="B53" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>214</v>
+      </c>
+      <c r="B54" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>214</v>
+      </c>
+      <c r="B55" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>214</v>
+      </c>
+      <c r="B56" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>214</v>
+      </c>
+      <c r="B57" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -5000,39 +5205,23 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B2:B55 B57:B5000</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{FDF76BD5-B98F-4973-BDBA-B75FF7A2BE62}">
-            <xm:f>AND(COUNTIF('Site Columns'!$B:$B,$B56)&lt;1,NOT(ISBLANK($B56)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FFFF0000"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFF7C80"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>B56</xm:sqref>
+          <xm:sqref>B2:B5000</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B49D0011-78F6-4D70-A75E-2F15AD9090AB}">
-          <x14:formula1>
-            <xm:f>OFFSET('Site Columns'!$B$2,0,0,COUNTA('Site Columns'!$B$2:$B$201))</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E26F9B81-88C7-4111-8D89-542FC41E1778}">
           <x14:formula1>
             <xm:f>OFFSET(Lists!$A$2,0,0,COUNTA(Lists!$A$2:$A$201))</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B49D0011-78F6-4D70-A75E-2F15AD9090AB}">
+          <x14:formula1>
+            <xm:f>OFFSET('Site Columns'!$B$2,0,0,COUNTA('Site Columns'!$B$2:$B$200))</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>